<commit_message>
added Jéröme Willems (SPW)
</commit_message>
<xml_diff>
--- a/ICEG-PersonList .xlsx
+++ b/ICEG-PersonList .xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc.bruyland\OneDrive - GCloud Belgium\Documents\WG_ICEG\ICEG presentations\REV_20191011\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcloudbelgium-my.sharepoint.com/personal/marc_bruyland_bosa_fgov_be/Documents/Documents/WG_ICEG/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{D706CA44-37CC-411A-9743-1F76DFE895DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{9E384B2C-6E1E-469D-A520-9ED3B5FA5706}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5D1EDE9-2F55-41A3-B122-15A610392CCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D3D7583-45EE-49AC-A828-9EBBA903D001}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$19:$A$6301</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$19:$A$6303</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="112">
   <si>
     <t>OU</t>
   </si>
@@ -359,6 +359,18 @@
   </si>
   <si>
     <t>rpereira@cirb.brussels</t>
+  </si>
+  <si>
+    <t>jerome.patrick.willems@spw.wallonie.be</t>
+  </si>
+  <si>
+    <t>Jérôme</t>
+  </si>
+  <si>
+    <t>Willems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPW = Service Public Wallonie </t>
   </si>
 </sst>
 </file>
@@ -497,12 +509,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74C0F28B-114B-490F-8EF4-0424BED04FA1}" name="Table1" displayName="Table1" ref="A1:E30" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E30" xr:uid="{57A42AF8-05CC-49D6-A904-FE89BF898683}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E30">
-    <sortCondition ref="A2:A30"/>
-    <sortCondition ref="B2:B30"/>
-    <sortCondition ref="C2:C30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74C0F28B-114B-490F-8EF4-0424BED04FA1}" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E31" xr:uid="{57A42AF8-05CC-49D6-A904-FE89BF898683}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">
+    <sortCondition ref="A2:A31"/>
+    <sortCondition ref="B2:B31"/>
+    <sortCondition ref="C2:C31"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C814016B-83D5-4C38-A191-6EDBFDDCDF23}" name="OU"/>
@@ -812,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F7E18D-9D32-40EF-A662-9ECA2F934D91}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +895,7 @@
         <v>84</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G30" si="0">IF(D3 &lt;&gt;"tbd", G2&amp;";"&amp;D3,G2)</f>
+        <f t="shared" ref="G3:G31" si="0">IF(D3 &lt;&gt;"tbd", G2&amp;";"&amp;D3,G2)</f>
         <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be</v>
       </c>
     </row>
@@ -1225,86 +1237,86 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>36</v>
+        <v>99</v>
+      </c>
+      <c r="B21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" t="s">
+        <v>109</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" t="s">
-        <v>33</v>
+        <v>108</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
+      <c r="B22" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>41</v>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" t="s">
         <v>33</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels </v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1312,104 +1324,104 @@
         <v>58</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels</v>
+        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels </v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be </v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="E28" t="s">
         <v>33</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be </v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>53</v>
+        <v>90</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1417,50 +1429,70 @@
         <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>53</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="315" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="315" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="5" t="str">
-        <f>G30</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
+      <c r="D34" s="5" t="str">
+        <f>G31</f>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" display="mailto:wim.bonneux@minfin.fed.be" xr:uid="{2433AB49-3546-47F5-B4BE-52BA6E657B1C}"/>
+    <hyperlink ref="D21" r:id="rId2" display="mailto:jerome.patrick.willems@spw.wallonie.be" xr:uid="{AAD259FE-B64C-42F3-8804-7115295182DF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1469,9 +1501,15 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004737C511A6E23947AD14508ECFA660DC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0dac2bd4b9910dbc7ba732ce23202609">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5b340481-ff30-4157-987a-05f8c1c3754a" xmlns:ns4="c1fa55ad-f680-4b5e-b0c5-c910667318ab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85b5d4cdc5a71fa11467f17736926f78" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004737C511A6E23947AD14508ECFA660DC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e35343c71a44f2b5b6a611bc8edcf0cf">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5b340481-ff30-4157-987a-05f8c1c3754a" xmlns:ns4="c1fa55ad-f680-4b5e-b0c5-c910667318ab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7b272f33889d15a62470ecb8934c9956" ns3:_="" ns4:_="">
     <xsd:import namespace="5b340481-ff30-4157-987a-05f8c1c3754a"/>
     <xsd:import namespace="c1fa55ad-f680-4b5e-b0c5-c910667318ab"/>
     <xsd:element name="properties">
@@ -1490,6 +1528,7 @@
                 <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1533,6 +1572,11 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="18" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -1673,23 +1717,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1453B941-BB20-4C76-8540-80BBC435E41D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="c1fa55ad-f680-4b5e-b0c5-c910667318ab"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5b340481-ff30-4157-987a-05f8c1c3754a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{407D0A84-4765-4B8B-8260-B6BFA4338C6E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1697,8 +1724,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1453B941-BB20-4C76-8540-80BBC435E41D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="c1fa55ad-f680-4b5e-b0c5-c910667318ab"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5b340481-ff30-4157-987a-05f8c1c3754a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9A45D31-968B-45E6-B89B-4586A18391BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E665B48A-972E-4F87-A577-05F7DD2A2A5D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>

</xml_diff>

<commit_message>
Marc Cools replaced by Stéphane Roberti
</commit_message>
<xml_diff>
--- a/ICEG-PersonList .xlsx
+++ b/ICEG-PersonList .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcloudbelgium-my.sharepoint.com/personal/marc_bruyland_bosa_fgov_be/Documents/Documents/WG_ICEG/Doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc.bruyland\OneDrive - GCloud Belgium\Documents\WG_ICEG\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5D1EDE9-2F55-41A3-B122-15A610392CCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{E5D1EDE9-2F55-41A3-B122-15A610392CCA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{0C01606F-287D-4302-9300-E384B3D6C026}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D3D7583-45EE-49AC-A828-9EBBA903D001}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="113">
   <si>
     <t>OU</t>
   </si>
@@ -244,12 +244,6 @@
     <t>LA VSGB/AVCB – Brulocalis</t>
   </si>
   <si>
-    <t>Cools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marc.cools@brulocalis.brussels </t>
-  </si>
-  <si>
     <t>LA VICTOR</t>
   </si>
   <si>
@@ -371,6 +365,15 @@
   </si>
   <si>
     <t xml:space="preserve">SPW = Service Public Wallonie </t>
+  </si>
+  <si>
+    <t>Roberti</t>
+  </si>
+  <si>
+    <t>Stephane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stephane.roberti@brulocalis.brussels </t>
   </si>
 </sst>
 </file>
@@ -826,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F7E18D-9D32-40EF-A662-9ECA2F934D91}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +868,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -874,7 +877,7 @@
         <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G2" t="str">
         <f>Table1[[#This Row],[e-mail]]</f>
@@ -883,7 +886,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -892,7 +895,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G31" si="0">IF(D3 &lt;&gt;"tbd", G2&amp;";"&amp;D3,G2)</f>
@@ -901,7 +904,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -922,7 +925,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -949,7 +952,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
@@ -964,13 +967,13 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -1021,19 +1024,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -1042,7 +1045,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
@@ -1054,7 +1057,7 @@
         <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -1063,19 +1066,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
         <v>71</v>
       </c>
-      <c r="B12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
         <v>73</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" t="s">
-        <v>75</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -1087,20 +1090,20 @@
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>70</v>
+        <v>111</v>
+      </c>
+      <c r="D13" t="s">
+        <v>112</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels </v>
+        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels </v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1117,16 +1120,16 @@
         <v>65</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
         <v>62</v>
@@ -1138,16 +1141,16 @@
         <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -1156,16 +1159,16 @@
         <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
@@ -1174,16 +1177,16 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -1192,16 +1195,16 @@
         <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -1210,16 +1213,16 @@
         <v>21</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>11</v>
@@ -1232,28 +1235,28 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1274,7 +1277,7 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1288,14 +1291,14 @@
         <v>39</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1309,14 +1312,14 @@
         <v>41</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1337,7 +1340,7 @@
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels </v>
+        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels </v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1345,20 +1348,20 @@
         <v>58</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" t="s">
         <v>105</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" t="s">
-        <v>107</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1372,14 +1375,14 @@
         <v>44</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1400,7 +1403,7 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be </v>
+        <v xml:space="preserve">raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be </v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1414,14 +1417,14 @@
         <v>46</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E29" t="s">
         <v>33</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1442,7 +1445,7 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1463,7 +1466,7 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1472,42 +1475,28 @@
     </row>
     <row r="34" spans="1:4" ht="315" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D34" s="5" t="str">
         <f>G31</f>
-        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;marc.cools@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
+        <v>raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;Thierry.BROUWER@cfwb.be;Thomas.aussems@dgov.be;godefroid.drugman@bosa.fgov.be;wim.bonneux@minfin.fed.be;raf.janssens@minfin.fed.be;frank.vandeheijning@minfin.fed.be;j.lambillotte@imio.be ;eddy.vds@v-ict-or.be;stephane.roberti@brulocalis.brussels ;david.mena@brulocalis.brussels;ward.vanhal@vvsg.be;fdumortier@cirb.brussels;ahof@cibg.brussels; ahof@gob.brussels;raf.buyle@kb.vlaanderen.be;ziggy.vanlishout@kb.vlaanderen.be;olivierpascal.bakasanda@ensemblesimplifions.be;jerome.patrick.willems@spw.wallonie.be;marc.bruyland@bosa.fgov.be;liesbet.dhondt@bosa.fgov.be;bart.hanssens@bosa.fgov.be;dlegrelle@cirb.brussels ;rpereira@cirb.brussels;Robin.Bosman@ehealth.fgov.be;tony.vanderstraete@kb.vlaanderen.be ;Peter.VanDenBosch@ksz-bcss.fgov.be;olivierpascal.bakasanda@ensemblesimplifions.be;cedric.jeanmart@ensemblesimplifions.be</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" display="mailto:wim.bonneux@minfin.fed.be" xr:uid="{2433AB49-3546-47F5-B4BE-52BA6E657B1C}"/>
     <hyperlink ref="D21" r:id="rId2" display="mailto:jerome.patrick.willems@spw.wallonie.be" xr:uid="{AAD259FE-B64C-42F3-8804-7115295182DF}"/>
+    <hyperlink ref="D13" r:id="rId3" xr:uid="{BB9E5810-FA6F-49E3-BD25-A46E3867192D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004737C511A6E23947AD14508ECFA660DC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e35343c71a44f2b5b6a611bc8edcf0cf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5b340481-ff30-4157-987a-05f8c1c3754a" xmlns:ns4="c1fa55ad-f680-4b5e-b0c5-c910667318ab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7b272f33889d15a62470ecb8934c9956" ns3:_="" ns4:_="">
     <xsd:import namespace="5b340481-ff30-4157-987a-05f8c1c3754a"/>
@@ -1716,32 +1705,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{407D0A84-4765-4B8B-8260-B6BFA4338C6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1453B941-BB20-4C76-8540-80BBC435E41D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="c1fa55ad-f680-4b5e-b0c5-c910667318ab"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5b340481-ff30-4157-987a-05f8c1c3754a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E665B48A-972E-4F87-A577-05F7DD2A2A5D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1758,4 +1737,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1453B941-BB20-4C76-8540-80BBC435E41D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5b340481-ff30-4157-987a-05f8c1c3754a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c1fa55ad-f680-4b5e-b0c5-c910667318ab"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{407D0A84-4765-4B8B-8260-B6BFA4338C6E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>